<commit_message>
Cheking breakpoints for responsive footer: heightness
</commit_message>
<xml_diff>
--- a/TAGS.xlsx
+++ b/TAGS.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="63" uniqueCount="31">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="93" uniqueCount="34">
   <si>
     <t>GRAPHIC</t>
   </si>
@@ -109,6 +109,15 @@
   </si>
   <si>
     <t>MARKUP</t>
+  </si>
+  <si>
+    <t>v</t>
+  </si>
+  <si>
+    <t>x</t>
+  </si>
+  <si>
+    <t>RESPONSIVE FOOTER HEIGHT</t>
   </si>
 </sst>
 </file>
@@ -456,16 +465,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:W10"/>
+  <dimension ref="A1:W29"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="P1" workbookViewId="0">
-      <selection activeCell="W1" sqref="W1"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="I21" sqref="I21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="19" customWidth="1"/>
-    <col min="2" max="2" width="24.5703125" customWidth="1"/>
+    <col min="1" max="2" width="35.28515625" customWidth="1"/>
     <col min="3" max="3" width="16" customWidth="1"/>
     <col min="4" max="4" width="25.85546875" customWidth="1"/>
     <col min="17" max="17" width="17.42578125" customWidth="1"/>
@@ -536,6 +544,12 @@
       <c r="U2" t="s">
         <v>28</v>
       </c>
+      <c r="V2" t="s">
+        <v>31</v>
+      </c>
+      <c r="W2" t="s">
+        <v>31</v>
+      </c>
     </row>
     <row r="3" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
@@ -553,6 +567,12 @@
       <c r="Q3" t="s">
         <v>24</v>
       </c>
+      <c r="V3" t="s">
+        <v>31</v>
+      </c>
+      <c r="W3" t="s">
+        <v>31</v>
+      </c>
     </row>
     <row r="4" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
@@ -582,6 +602,12 @@
       <c r="S4" t="s">
         <v>26</v>
       </c>
+      <c r="V4" t="s">
+        <v>31</v>
+      </c>
+      <c r="W4" t="s">
+        <v>31</v>
+      </c>
     </row>
     <row r="5" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
@@ -623,6 +649,12 @@
       <c r="U5" t="s">
         <v>28</v>
       </c>
+      <c r="V5" t="s">
+        <v>31</v>
+      </c>
+      <c r="W5" t="s">
+        <v>31</v>
+      </c>
     </row>
     <row r="6" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
@@ -631,6 +663,12 @@
       <c r="F6" t="s">
         <v>13</v>
       </c>
+      <c r="V6" t="s">
+        <v>31</v>
+      </c>
+      <c r="W6" t="s">
+        <v>31</v>
+      </c>
     </row>
     <row r="7" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
@@ -654,11 +692,23 @@
       <c r="U7" t="s">
         <v>28</v>
       </c>
+      <c r="V7" t="s">
+        <v>31</v>
+      </c>
+      <c r="W7" t="s">
+        <v>31</v>
+      </c>
     </row>
     <row r="8" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>6</v>
       </c>
+      <c r="V8" t="s">
+        <v>31</v>
+      </c>
+      <c r="W8" t="s">
+        <v>31</v>
+      </c>
     </row>
     <row r="9" spans="1:23" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
@@ -670,6 +720,12 @@
       <c r="S9" t="s">
         <v>26</v>
       </c>
+      <c r="V9" t="s">
+        <v>31</v>
+      </c>
+      <c r="W9" t="s">
+        <v>31</v>
+      </c>
     </row>
     <row r="10" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
@@ -680,6 +736,134 @@
       </c>
       <c r="N10" t="s">
         <v>21</v>
+      </c>
+    </row>
+    <row r="12" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="A12" s="1"/>
+    </row>
+    <row r="19" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A19" s="1" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="21" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
+        <v>0</v>
+      </c>
+      <c r="B21">
+        <v>17</v>
+      </c>
+      <c r="H21">
+        <v>1280</v>
+      </c>
+    </row>
+    <row r="22" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
+        <v>1</v>
+      </c>
+      <c r="B22">
+        <v>4</v>
+      </c>
+      <c r="C22">
+        <v>480</v>
+      </c>
+      <c r="D22">
+        <v>640</v>
+      </c>
+    </row>
+    <row r="23" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A23" t="s">
+        <v>2</v>
+      </c>
+      <c r="B23">
+        <v>8</v>
+      </c>
+      <c r="D23">
+        <v>640</v>
+      </c>
+      <c r="E23">
+        <v>768</v>
+      </c>
+      <c r="G23">
+        <v>1024</v>
+      </c>
+      <c r="H23">
+        <v>1280</v>
+      </c>
+    </row>
+    <row r="24" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A24" t="s">
+        <v>3</v>
+      </c>
+      <c r="B24">
+        <v>12</v>
+      </c>
+      <c r="H24">
+        <v>1280</v>
+      </c>
+    </row>
+    <row r="25" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A25" t="s">
+        <v>4</v>
+      </c>
+      <c r="B25">
+        <v>1</v>
+      </c>
+      <c r="C25" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="26" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A26" t="s">
+        <v>5</v>
+      </c>
+      <c r="B26">
+        <v>6</v>
+      </c>
+      <c r="C26">
+        <v>480</v>
+      </c>
+      <c r="D26">
+        <v>640</v>
+      </c>
+      <c r="E26">
+        <v>768</v>
+      </c>
+      <c r="F26">
+        <v>800</v>
+      </c>
+    </row>
+    <row r="27" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A27" t="s">
+        <v>6</v>
+      </c>
+      <c r="B27">
+        <v>1</v>
+      </c>
+      <c r="C27" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="28" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A28" t="s">
+        <v>7</v>
+      </c>
+      <c r="B28">
+        <v>2</v>
+      </c>
+      <c r="C28" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="29" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A29" t="s">
+        <v>8</v>
+      </c>
+      <c r="B29">
+        <v>2</v>
+      </c>
+      <c r="C29" t="s">
+        <v>32</v>
       </c>
     </row>
   </sheetData>

</xml_diff>